<commit_message>
added csvs, zip, updated report
</commit_message>
<xml_diff>
--- a/proj02/csvs/datums.xlsx
+++ b/proj02/csvs/datums.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Validation</t>
   </si>
@@ -27,10 +27,10 @@
     <t>Window size 5</t>
   </si>
   <si>
-    <t>def?</t>
+    <t>def1</t>
   </si>
   <si>
-    <t>def1</t>
+    <t>Baseline</t>
   </si>
   <si>
     <t>Window size</t>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Soft-scoring</t>
-  </si>
-  <si>
-    <t>Baseline</t>
   </si>
   <si>
     <t>Without examples and without wordnetInts</t>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>1, 4, 5</t>
+  </si>
+  <si>
+    <t>Window size 8, eq w, with everything, def 1</t>
   </si>
   <si>
     <t>1, 6, 3</t>
@@ -224,10 +224,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B15" activeCellId="0" pane="topLeft" sqref="B15"/>
+      <selection activeCell="C22" activeCellId="0" pane="topLeft" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -257,10 +257,10 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -281,77 +281,95 @@
       <c r="J2" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="K2" s="0" t="n">
+        <v>0.54186</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.54126</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>0.33112</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0.54186</v>
+        <v>0.35681</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.33112</v>
+        <v>0.36763</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="J4" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>0.35681</v>
+        <v>0.41348</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.446528</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0.36763</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="J5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.41348</v>
+        <v>0.39051</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
@@ -359,138 +377,138 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.446528</v>
+        <v>0.431939</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="K6" s="0" t="n">
-        <v>0.39051</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>0.431939</v>
-      </c>
+        <v>0.43287</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="D7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="K7" s="0" t="n">
-        <v>0.43287</v>
+        <v>0.43492</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="D8" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.4367</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="E9" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="H8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>0.43492</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="D9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>12</v>
-      </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>0.4367</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+        <v>0.44181</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>4</v>
+      <c r="B10" s="0" t="n">
+        <v>0.32904</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0.44181</v>
+        <v>0.44283</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
@@ -498,283 +516,349 @@
         <v>22</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.32904</v>
+        <v>0.35798</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>20</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0.44283</v>
+        <v>0.45202</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.44587</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>0.35798</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="G12" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>0.45202</v>
+        <v>0.43134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>0.44587</v>
+        <v>0.43301</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>0.43134</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.43301</v>
-      </c>
+        <v>0.44666</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="D14" s="0" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="I14" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>0.44666</v>
+        <v>0.4367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="D15" s="0" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.43221</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.4523</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>14</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>0.4367</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
-      <c r="D16" s="0" t="n">
-        <v>11</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>0.43221</v>
+        <v>0.42926</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
       <c r="D17" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0.42926</v>
+        <v>0.43287</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="D18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="I18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0.43287</v>
+        <v>0.43849</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="D19" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0.43849</v>
+        <v>0.43083</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
-      <c r="D20" s="0" t="n">
-        <v>13</v>
-      </c>
       <c r="E20" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>0.43083</v>
+        <v>0.35911</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="E21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.38617</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+      <c r="E22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.44564</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="E23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.45559</v>
       </c>
     </row>
   </sheetData>
@@ -793,10 +877,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L934"/>
+  <dimension ref="A1:J934"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A931" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H961" activeCellId="0" pane="topLeft" sqref="H961"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="J13" activeCellId="0" pane="topLeft" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -900,10 +984,6 @@
         <f aca="false">IF(E3= A3)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="0" t="e">
-        <f aca="false">COUNTIF(G2:G933, =1)</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">

</xml_diff>